<commit_message>
UI Testing : Personal Detail's Page UI Check Test.
Evidence attached, data provider installed.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{702635AB-9030-4F88-9B5C-C717FB553DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC105425-DDF7-428B-8BDB-821A4FAEB643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T_LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="T_MyInfoPDUITest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Case_ID</t>
   </si>
@@ -70,6 +71,78 @@
   </si>
   <si>
     <t>Login Successful</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Status Expected</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Case_005</t>
+  </si>
+  <si>
+    <t>OtherId</t>
+  </si>
+  <si>
+    <t>Case_006</t>
+  </si>
+  <si>
+    <t>Driver License Number</t>
+  </si>
+  <si>
+    <t>Case_007</t>
+  </si>
+  <si>
+    <t>License Expiry Date</t>
+  </si>
+  <si>
+    <t>Case_008</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Case_009</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Case_010</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Case_011</t>
+  </si>
+  <si>
+    <t>Male Checkbox</t>
+  </si>
+  <si>
+    <t>Case_012</t>
+  </si>
+  <si>
+    <t>Female Checkbox</t>
   </si>
 </sst>
 </file>
@@ -127,7 +200,122 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -138,6 +326,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F7BBBD4-5B71-4DE8-8DE4-D84586F2E906}" name="Table1" displayName="Table1" ref="B1:C13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="B1:C13" xr:uid="{8F7BBBD4-5B71-4DE8-8DE4-D84586F2E906}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{39C9FE51-4D67-4EDE-8677-214F0AFD1893}" name="Field" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2D489B7B-A6E8-42B4-B0FF-9DD29DF670D9}" name="Status Expected" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,4 +743,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CA885A-1669-46CB-80D8-2A3609659983}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Functionality : Update of Personal Details.
Learn : Custom wait Excepted condition. Override apply method.
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC105425-DDF7-428B-8BDB-821A4FAEB643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0156789B-297C-451E-B097-175A1D3BB559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T_LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="T_MyInfoPDUITest" sheetId="2" r:id="rId2"/>
+    <sheet name="T_PersonalDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>Case_ID</t>
   </si>
@@ -79,70 +80,118 @@
     <t>Status Expected</t>
   </si>
   <si>
+    <t>Case_005</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
     <t>Enable</t>
   </si>
   <si>
+    <t>Case_006</t>
+  </si>
+  <si>
     <t>MiddleName</t>
   </si>
   <si>
+    <t>Case_007</t>
+  </si>
+  <si>
     <t>LastName</t>
   </si>
   <si>
+    <t>Case_008</t>
+  </si>
+  <si>
     <t>EmployeeId</t>
   </si>
   <si>
     <t>Disable</t>
   </si>
   <si>
-    <t>Case_005</t>
+    <t>Case_009</t>
   </si>
   <si>
     <t>OtherId</t>
   </si>
   <si>
-    <t>Case_006</t>
+    <t>Case_010</t>
   </si>
   <si>
     <t>Driver License Number</t>
   </si>
   <si>
-    <t>Case_007</t>
+    <t>Case_011</t>
   </si>
   <si>
     <t>License Expiry Date</t>
   </si>
   <si>
-    <t>Case_008</t>
+    <t>Case_012</t>
   </si>
   <si>
     <t>Nationality</t>
   </si>
   <si>
-    <t>Case_009</t>
+    <t>Case_013</t>
   </si>
   <si>
     <t>Marital Status</t>
   </si>
   <si>
-    <t>Case_010</t>
+    <t>Case_014</t>
   </si>
   <si>
     <t>Date Of Birth</t>
   </si>
   <si>
-    <t>Case_011</t>
+    <t>Case_015</t>
   </si>
   <si>
     <t>Male Checkbox</t>
   </si>
   <si>
-    <t>Case_012</t>
+    <t>Case_016</t>
   </si>
   <si>
     <t>Female Checkbox</t>
+  </si>
+  <si>
+    <t>Update Field</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Case_017</t>
+  </si>
+  <si>
+    <t>Saurabh</t>
+  </si>
+  <si>
+    <t>Updated Successfully</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Kutwal</t>
+  </si>
+  <si>
+    <t>112451</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>2000-03-19</t>
   </si>
 </sst>
 </file>
@@ -166,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -189,18 +238,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -329,11 +529,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F7BBBD4-5B71-4DE8-8DE4-D84586F2E906}" name="Table1" displayName="Table1" ref="B1:C13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F7BBBD4-5B71-4DE8-8DE4-D84586F2E906}" name="Table1" displayName="Table1" ref="B1:C13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="B1:C13" xr:uid="{8F7BBBD4-5B71-4DE8-8DE4-D84586F2E906}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{39C9FE51-4D67-4EDE-8677-214F0AFD1893}" name="Field" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{2D489B7B-A6E8-42B4-B0FF-9DD29DF670D9}" name="Status Expected" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{39C9FE51-4D67-4EDE-8677-214F0AFD1893}" name="Field" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2D489B7B-A6E8-42B4-B0FF-9DD29DF670D9}" name="Status Expected" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57BA0F12-E643-4652-A208-CC9B5D27D587}" name="Table2" displayName="Table2" ref="B1:D9" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="B1:D9" xr:uid="{57BA0F12-E643-4652-A208-CC9B5D27D587}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CDB53555-895B-4CCA-B965-C93DE16D2AD6}" name="Update Field" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{5C1C8FEE-4699-4CDB-915C-0905DCC2B984}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2B820F07-F6E3-4ACB-A855-751C8836E01B}" name="Expected" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -659,7 +871,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -749,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CA885A-1669-46CB-80D8-2A3609659983}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,134 +984,270 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB895EA-F2B1-45E4-A891-D8A55A64F348}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>